<commit_message>
simple ai agent finished
</commit_message>
<xml_diff>
--- a/app/entrada.xlsx
+++ b/app/entrada.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>consulta</t>
+  </si>
+  <si>
+    <t>Zoom Video Communications</t>
+  </si>
+  <si>
+    <t>ZOTAC</t>
+  </si>
+  <si>
+    <t>Zuken</t>
   </si>
   <si>
     <t>Don Best Sports</t>
@@ -383,31 +392,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2">
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>